<commit_message>
add bulk upload file to project
</commit_message>
<xml_diff>
--- a/src/main/resources/public/employee_bulk_upload.xlsx
+++ b/src/main/resources/public/employee_bulk_upload.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MikeHenry\srv\applications\kotlinApps\kotlin-playground\src\main\resources\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -124,13 +129,16 @@
   </si>
   <si>
     <t>Chesa</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,11 +186,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -190,6 +199,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -236,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,9 +285,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,6 +320,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,29 +496,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,440 +527,470 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4">
+        <v>32874</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4">
+        <v>33605</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
       <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
       <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4">
+        <v>33606</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
       <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4">
+        <v>33973</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
       <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
       <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4">
+        <v>34339</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
       <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
       <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4">
+        <v>34705</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
       <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
       <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4">
+        <v>35071</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
       <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
       <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4">
+        <v>35438</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
       <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
       <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4">
+        <v>35804</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
       <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
         <v>18</v>
       </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
       <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="3"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -948,26 +998,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>